<commit_message>
POM and Config file Upadated
</commit_message>
<xml_diff>
--- a/TestDataFiles/TestcaseReport_Dashboard.xlsx
+++ b/TestDataFiles/TestcaseReport_Dashboard.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="233">
   <si>
     <t>Test case description</t>
   </si>
@@ -991,6 +991,66 @@
   </si>
   <si>
     <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\monthPerformance_19_06_2023_11_18_54.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\monthPerformance_19_06_2023_14_29_28.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\lowAttendancePerformance_19_06_2023_14_30_26.png</t>
+  </si>
+  <si>
+    <t>CP-28</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\GirdPerformance_19_06_2023_14_31_23.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\characteristicPerformance_19_06_2023_14_31_27.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\Marks_Obtained_19_06_2023_14_31_31.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\total_Marks_19_06_2023_14_31_34.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\marks_Percentage_19_06_2023_14_31_38.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\attendance_Percentage_19_06_2023_14_31_42.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\Group_Marking_19_06_2023_14_31_45.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\monthPerformance_19_06_2023_14_35_40.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\lowAttendancePerformance_19_06_2023_14_36_36.png</t>
+  </si>
+  <si>
+    <t>CP-29</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\GirdPerformance_19_06_2023_14_37_33.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\characteristicPerformance_19_06_2023_14_37_37.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\Marks_Obtained_19_06_2023_14_37_41.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\total_Marks_19_06_2023_14_37_45.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\marks_Percentage_19_06_2023_14_37_49.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\attendance_Percentage_19_06_2023_14_37_53.png</t>
+  </si>
+  <si>
+    <t>G:\E_Git_Traingings_Ecplise_workspace\E_POC2\Screenshots\Group_Marking_19_06_2023_14_37_56.png</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1646,7 @@
         <v>186</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="14" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -1618,10 +1678,10 @@
         <v>189</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="409.5" x14ac:dyDescent="0.25">
@@ -1656,7 +1716,7 @@
         <v>186</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>193</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -1691,7 +1751,7 @@
         <v>186</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -1726,7 +1786,7 @@
         <v>186</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>197</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -1761,7 +1821,7 @@
         <v>186</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -1796,7 +1856,7 @@
         <v>186</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>201</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1831,7 +1891,7 @@
         <v>186</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -1866,7 +1926,7 @@
         <v>186</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>